<commit_message>
Updated resistor supplier number
* Resistor supplier part number was misspelled
</commit_message>
<xml_diff>
--- a/PIC32ETH/Project_Outputs/Bill_Of_Materials/Bill_Of_Materials.xlsx
+++ b/PIC32ETH/Project_Outputs/Bill_Of_Materials/Bill_Of_Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PIC32ETH_EL\PIC32ETH\Project_Outputs\Bill_Of_Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F022767-3B73-45EF-9505-1BD1E816F445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2D44700-8FC7-495F-BD87-B78442DA4816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="5025" windowWidth="18690" windowHeight="15435" xr2:uid="{A67C6AE3-BF04-41B9-BBC8-CBF3D9D2D108}"/>
+    <workbookView xWindow="0" yWindow="3580" windowWidth="19200" windowHeight="9993" xr2:uid="{DF08DFF5-2991-4AA5-93C0-6F667A6F3D15}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill_Of_Materials" sheetId="1" r:id="rId1"/>
@@ -914,7 +914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F931B051-98D9-469F-A5D9-1E68E2A8E3E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064CA40D-47E0-4F35-8A7A-81D2D8B50916}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -922,17 +922,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.87890625" customWidth="1"/>
+    <col min="2" max="2" width="27.76171875" customWidth="1"/>
+    <col min="3" max="3" width="23.3515625" customWidth="1"/>
+    <col min="4" max="4" width="41.29296875" customWidth="1"/>
+    <col min="5" max="5" width="28.64453125" customWidth="1"/>
+    <col min="6" max="6" width="18.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -952,7 +952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -972,7 +972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -992,7 +992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
         <v>40</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
         <v>47</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
         <v>51</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="s">
         <v>58</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="s">
         <v>61</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="s">
         <v>64</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="s">
         <v>70</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
         <v>75</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="s">
         <v>79</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="s">
         <v>83</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="s">
         <v>91</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="s">
         <v>95</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="s">
         <v>103</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="s">
         <v>107</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="s">
         <v>111</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="s">
         <v>115</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="s">
         <v>119</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="s">
         <v>123</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="s">
         <v>127</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
         <v>131</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="s">
         <v>134</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="s">
         <v>137</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="s">
         <v>141</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="s">
         <v>145</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="s">
         <v>149</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="s">
         <v>153</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="s">
         <v>157</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="s">
         <v>161</v>
       </c>
@@ -1775,6 +1775,6 @@
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="72" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>